<commit_message>
CAMBIOS DE SINDICATO POR sindicao
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
@@ -5531,10 +5531,10 @@
   <dimension ref="A3:DV6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="CO5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="BY5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="CP4" sqref="CP4"/>
+      <selection pane="bottomRight" activeCell="CE5" sqref="CE5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6224,7 +6224,8 @@
         <v>82</v>
       </c>
       <c r="CE5" s="60">
-        <v>83</v>
+        <f>BW5+BY5+BZ5+CA5+CB5+CC5+CD5-BT5-BU5-BV5</f>
+        <v>333</v>
       </c>
       <c r="CF5" s="60">
         <v>84</v>

</xml_diff>

<commit_message>
CAMBIOS DE FINIQUITO, GUARDAR INDIVIDUALMENTE git add -A
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/TMM.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1199" uniqueCount="439">
   <si>
     <t>TOTAL</t>
   </si>
@@ -1310,15 +1310,9 @@
     <t>VEJEZ</t>
   </si>
   <si>
-    <t>REPORTE DE LA NÓMINA</t>
-  </si>
-  <si>
     <t>Nomina:</t>
   </si>
   <si>
-    <t>Clasificacion:</t>
-  </si>
-  <si>
     <t xml:space="preserve">Periodo de pago: </t>
   </si>
   <si>
@@ -1368,6 +1362,9 @@
   </si>
   <si>
     <t>TIEMPO EXTRA TRIPLE</t>
+  </si>
+  <si>
+    <t>Reporte de Nómina</t>
   </si>
 </sst>
 </file>
@@ -3272,7 +3269,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -3394,7 +3391,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -3429,6 +3425,9 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1493">
     <cellStyle name="Comma_2 SALARIOS" xfId="1491"/>
@@ -7216,19 +7215,19 @@
       <c r="F2" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="G2" s="73"/>
-      <c r="H2" s="74"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="73"/>
     </row>
     <row r="3" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="75" t="str">
+      <c r="B3" s="74" t="str">
         <f>+CONCATENATE("FACTURA ",G2)</f>
         <v xml:space="preserve">FACTURA </v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="F3" s="77" t="s">
+      <c r="C3" s="75"/>
+      <c r="F3" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="77"/>
+      <c r="G3" s="76"/>
       <c r="H3" s="44">
         <v>0</v>
       </c>
@@ -7241,10 +7240,10 @@
         <f>+H8</f>
         <v>empresa</v>
       </c>
-      <c r="F4" s="78" t="s">
+      <c r="F4" s="77" t="s">
         <v>99</v>
       </c>
-      <c r="G4" s="79"/>
+      <c r="G4" s="78"/>
       <c r="H4" s="44">
         <v>0</v>
       </c>
@@ -7257,10 +7256,10 @@
         <f>+H4+H5+H6+H7</f>
         <v>0</v>
       </c>
-      <c r="F5" s="78" t="s">
+      <c r="F5" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="79"/>
+      <c r="G5" s="78"/>
       <c r="H5" s="44">
         <v>0</v>
       </c>
@@ -7273,10 +7272,10 @@
         <f>+C5</f>
         <v>0</v>
       </c>
-      <c r="F6" s="80" t="s">
+      <c r="F6" s="79" t="s">
         <v>101</v>
       </c>
-      <c r="G6" s="80"/>
+      <c r="G6" s="79"/>
       <c r="H6" s="44">
         <v>0</v>
       </c>
@@ -7309,10 +7308,10 @@
         <f>+C6+C7</f>
         <v>0</v>
       </c>
-      <c r="F8" s="72" t="s">
+      <c r="F8" s="71" t="s">
         <v>103</v>
       </c>
-      <c r="G8" s="72"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="56" t="s">
         <v>106</v>
       </c>
@@ -10227,219 +10226,212 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F45"/>
+  <dimension ref="A2:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="18" x14ac:dyDescent="0.25">
-      <c r="B2" s="81" t="s">
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.25">
+      <c r="B2" s="80" t="s">
+        <v>438</v>
+      </c>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="65"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="81" t="s">
         <v>420</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="65"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="67" t="s">
+      <c r="B4" s="82"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="81" t="s">
         <v>421</v>
       </c>
-      <c r="B4" s="66"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="67" t="s">
+      <c r="B5" s="82"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="81" t="s">
         <v>422</v>
       </c>
-      <c r="B5" s="66"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="67" t="s">
+      <c r="B6" s="82"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="D7" s="67" t="s">
         <v>423</v>
       </c>
-      <c r="B6" s="66"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="67" t="s">
+      <c r="E7" t="s">
         <v>424</v>
       </c>
-      <c r="B7" s="66"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E8" s="68" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B10" s="70" t="s">
         <v>425</v>
       </c>
-      <c r="F8" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C23" s="70" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C11" s="71" t="s">
+      <c r="D23" s="69"/>
+      <c r="E23" s="66">
+        <f>+SUM(E12:E22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B25" s="83" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>437</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>432</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D24" s="70" t="s">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C40" s="83" t="s">
         <v>428</v>
       </c>
-      <c r="E24" s="70"/>
-      <c r="F24" s="66">
-        <f>+SUM(F13:F23)</f>
+      <c r="D40" s="68"/>
+      <c r="E40" s="66">
+        <f>+SUM(E27:E39)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C26" s="69" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B44" s="60" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="D41" s="69" t="s">
-        <v>430</v>
-      </c>
-      <c r="E41" s="69"/>
-      <c r="F41" s="66">
-        <f>+SUM(F28:F40)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C45" s="60" t="s">
-        <v>431</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>